<commit_message>
updated for the new bus routes
</commit_message>
<xml_diff>
--- a/BUS DATA.xlsx
+++ b/BUS DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\NUS\Orbital\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\Schedule-Buzzers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2763AC76-3A85-4AE1-94F3-D8B62C43A101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472D0066-3168-4260-BAB5-9FD1220A9077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4224" yWindow="2856" windowWidth="17280" windowHeight="8964" xr2:uid="{20FAF3BD-F824-4C96-AF4B-8D3EECA603AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20FAF3BD-F824-4C96-AF4B-8D3EECA603AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="122">
   <si>
     <t>A1</t>
   </si>
@@ -238,16 +238,182 @@
   </si>
   <si>
     <t>AS5,COM2</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Location:</t>
+  </si>
+  <si>
+    <t>Stop:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA1 </t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Opp NUSS, COM2, Ventus, CLB, LT13, AS5</t>
+  </si>
+  <si>
+    <t>E3, E4,E5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YIH, CLB, </t>
+  </si>
+  <si>
+    <t>AA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT, Opp YIH, YIH, CLB, </t>
+  </si>
+  <si>
+    <t>Opp HSSML, BIZ2</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>LT27, S17</t>
+  </si>
+  <si>
+    <t>Science Dr</t>
+  </si>
+  <si>
+    <t>Uhall, Opp Uhall</t>
+  </si>
+  <si>
+    <t>DD1</t>
+  </si>
+  <si>
+    <t>DD2</t>
+  </si>
+  <si>
+    <t>CCX</t>
+  </si>
+  <si>
+    <t>Music sch</t>
+  </si>
+  <si>
+    <t>Museum, Utown walk</t>
+  </si>
+  <si>
+    <t>Utown walk</t>
+  </si>
+  <si>
+    <t>Utown wak</t>
+  </si>
+  <si>
+    <t>Utwon walk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Med, den, </t>
+  </si>
+  <si>
+    <t>Nursing</t>
+  </si>
+  <si>
+    <t>EA, Raffles hall (opp Museum)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KR, Opp KR </t>
+  </si>
+  <si>
+    <t>Opp KR</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>BTC (start)</t>
+  </si>
+  <si>
+    <t>BTC(end)</t>
+  </si>
+  <si>
+    <t>PGP</t>
+  </si>
+  <si>
+    <t>PGPR (end)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGP </t>
+  </si>
+  <si>
+    <t>RVRC</t>
+  </si>
+  <si>
+    <t>Opp UHC, YIH, UHC</t>
+  </si>
+  <si>
+    <t>Opp UHC, UHC</t>
+  </si>
+  <si>
+    <t>Uhall, Opp UHC, UHC, Opp Uhall</t>
+  </si>
+  <si>
+    <t>YIH, Opp YIH (walking required)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School of public policy </t>
+  </si>
+  <si>
+    <t>Com2</t>
+  </si>
+  <si>
+    <t>TCOMS</t>
+  </si>
+  <si>
+    <t>TCOMS, Opp TCOMS</t>
+  </si>
+  <si>
+    <t>SDE</t>
+  </si>
+  <si>
+    <t>AA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLB(walk) </t>
+  </si>
+  <si>
+    <t>IT (walk)</t>
+  </si>
+  <si>
+    <t>Ventus, IT, CLB, LT13</t>
+  </si>
+  <si>
+    <t>USP</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>Public health</t>
+  </si>
+  <si>
+    <t>BB - Uhall, Opp Uhall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,8 +439,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A268FF2F-678F-400A-8403-9524FD783E09}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,9 +768,11 @@
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,56 +782,113 @@
       <c r="C1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -671,80 +898,158 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -754,72 +1059,135 @@
       <c r="C18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -829,48 +1197,90 @@
       <c r="C27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>24</v>
       </c>
       <c r="C30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -880,64 +1290,118 @@
       <c r="C33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>41</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>8</v>
       </c>
@@ -945,7 +1409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -955,40 +1419,79 @@
       <c r="C42" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>33</v>
       </c>
       <c r="C45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>35</v>
       </c>
       <c r="C46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>24</v>
       </c>
@@ -996,7 +1499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -1004,15 +1507,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>32</v>
       </c>
@@ -1020,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1031,17 +1540,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1558,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>24</v>
       </c>
@@ -1057,7 +1566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1574,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>24</v>
       </c>
@@ -1089,7 +1598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>53</v>
       </c>
@@ -1097,7 +1606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>16</v>
       </c>
@@ -1105,7 +1614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -1116,7 +1625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>37</v>
       </c>
@@ -1124,7 +1633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>9</v>
       </c>
@@ -1303,5 +1812,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>